<commit_message>
City index 25-11 9/12 WIP
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_20952.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_20952.xlsx
@@ -10,6 +10,7 @@
     <sheet name="punkt_adt" sheetId="1" r:id="rId1"/>
     <sheet name="punktindeks_maned" sheetId="2" r:id="rId2"/>
     <sheet name="byindeks_aarlig" sheetId="3" r:id="rId3"/>
+    <sheet name="byindeks_hittil" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -2385,7 +2386,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2467,2671 +2468,1291 @@
           <t>nov</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>des</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>24062V3324514</t>
+          <t>74674V248962</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Borge skole</t>
+          <t>Avkjøring Ålesundstunnelene V</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>fv. 130</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D2">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E2">
-        <v>-8.869999999999999</v>
+        <v>3.34</v>
       </c>
       <c r="F2">
-        <v>-3.3</v>
+        <v>5.02</v>
       </c>
       <c r="G2">
-        <v>-4.79</v>
+        <v>6.52</v>
       </c>
       <c r="H2">
-        <v>2.95</v>
+        <v>1.61</v>
       </c>
       <c r="I2">
-        <v>-0.08</v>
+        <v>1.18</v>
       </c>
       <c r="J2">
-        <v>-5.3</v>
+        <v>0.17</v>
       </c>
       <c r="K2">
-        <v>-3.26</v>
+        <v>10.31</v>
       </c>
       <c r="L2">
-        <v>-1.07</v>
+        <v>6.39</v>
       </c>
       <c r="M2">
-        <v>-1.71</v>
+        <v>7</v>
       </c>
       <c r="N2">
-        <v>0.92</v>
+        <v>6.2</v>
       </c>
       <c r="O2">
-        <v>1.42</v>
-      </c>
-      <c r="P2">
-        <v>7.54</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24062V3324514</t>
+          <t>14260V248961</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Borge skole</t>
+          <t>Avkjøring Ålesundstunnelene Ø</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fv. 130</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D3">
         <v>2025</v>
       </c>
       <c r="E3">
-        <v>10.4</v>
+        <v>2.53</v>
       </c>
       <c r="F3">
-        <v>4.91</v>
+        <v>2.95</v>
       </c>
       <c r="G3">
-        <v>5.9</v>
+        <v>4.81</v>
       </c>
       <c r="H3">
-        <v>2.73</v>
+        <v>-2.06</v>
       </c>
       <c r="I3">
-        <v>-0.62</v>
+        <v>1.21</v>
       </c>
       <c r="J3">
-        <v>0.35</v>
+        <v>1.3</v>
       </c>
       <c r="K3">
-        <v>5.22</v>
+        <v>7.43</v>
       </c>
       <c r="L3">
-        <v>1.24</v>
+        <v>1.03</v>
       </c>
       <c r="M3">
-        <v>-0.44</v>
+        <v>2.53</v>
       </c>
       <c r="N3">
-        <v>0.68</v>
+        <v>0.12</v>
+      </c>
+      <c r="O3">
+        <v>-1.96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>29444V971469</t>
+          <t>13279V248971</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fredrikstad bru vest</t>
+          <t>Blindheim øst</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>rv. 110</t>
+          <t>fv. 60</t>
         </is>
       </c>
       <c r="D4">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E4">
-        <v>3.4</v>
+        <v>3.43</v>
       </c>
       <c r="F4">
-        <v>6.01</v>
+        <v>2.53</v>
       </c>
       <c r="G4">
-        <v>-2.66</v>
+        <v>6.26</v>
       </c>
       <c r="H4">
-        <v>6.58</v>
+        <v>-2.34</v>
       </c>
       <c r="I4">
-        <v>0.19</v>
+        <v>2.14</v>
       </c>
       <c r="J4">
-        <v>-6.19</v>
+        <v>1.15</v>
       </c>
       <c r="K4">
-        <v>-5.89</v>
+        <v>4.64</v>
       </c>
       <c r="L4">
-        <v>-3.32</v>
+        <v>0.02</v>
       </c>
       <c r="M4">
-        <v>-4.6</v>
+        <v>3.04</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0.55</v>
       </c>
       <c r="O4">
-        <v>-0.38</v>
-      </c>
-      <c r="P4">
-        <v>1.57</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>29444V971469</t>
+          <t>78164V249524</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fredrikstad bru vest</t>
+          <t>Blindheimstunnelen</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>rv. 110</t>
+          <t>E39</t>
         </is>
       </c>
       <c r="D5">
         <v>2025</v>
       </c>
       <c r="E5">
-        <v>0.02</v>
+        <v>2.64</v>
       </c>
       <c r="F5">
-        <v>-2.64</v>
+        <v>3.38</v>
       </c>
       <c r="G5">
-        <v>4.8</v>
+        <v>5.22</v>
       </c>
       <c r="H5">
-        <v>-0.65</v>
+        <v>-2.86</v>
       </c>
       <c r="I5">
-        <v>0.61</v>
+        <v>4.1</v>
       </c>
       <c r="J5">
-        <v>5.38</v>
+        <v>-0.33</v>
       </c>
       <c r="K5">
-        <v>3.82</v>
+        <v>2.54</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="M5">
-        <v>1.69</v>
+        <v>1.76</v>
       </c>
       <c r="N5">
-        <v>0.53</v>
+        <v>-1.11</v>
+      </c>
+      <c r="O5">
+        <v>-1.82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>47762V971800</t>
+          <t>60191V249430</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fylkeshuset</t>
+          <t>Borgundgavelen</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fv. 109</t>
+          <t>fv. 536</t>
         </is>
       </c>
       <c r="D6">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E6">
-        <v>-3.94</v>
+        <v>-5.38</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>-3.03</v>
       </c>
       <c r="G6">
-        <v>-13.09</v>
+        <v>-2.37</v>
       </c>
       <c r="H6">
-        <v>8.109999999999999</v>
+        <v>-11.48</v>
       </c>
       <c r="I6">
-        <v>13.72</v>
+        <v>-3.43</v>
+      </c>
+      <c r="J6">
+        <v>-0.75</v>
       </c>
       <c r="K6">
-        <v>-4.44</v>
+        <v>1.93</v>
       </c>
       <c r="L6">
-        <v>-1.9</v>
-      </c>
-      <c r="M6">
-        <v>-6.19</v>
-      </c>
-      <c r="P6">
-        <v>3.86</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>47762V971800</t>
+          <t>91512V248948</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fylkeshuset</t>
+          <t>Borgundvegen</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fv. 109</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D7">
         <v>2025</v>
       </c>
       <c r="E7">
-        <v>-0.38</v>
+        <v>-0.29</v>
       </c>
       <c r="F7">
-        <v>-4.68</v>
+        <v>1.59</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>-8.94</v>
+      </c>
+      <c r="J7">
+        <v>-2.47</v>
+      </c>
+      <c r="K7">
+        <v>-2.14</v>
       </c>
       <c r="L7">
-        <v>-5.16</v>
-      </c>
-      <c r="M7">
-        <v>3.11</v>
+        <v>-0.99</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>69356V971439</t>
+          <t>16231V249213</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Glemmen</t>
+          <t>Brauta</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>fv. 109</t>
+          <t>fv. 5946</t>
         </is>
       </c>
       <c r="D8">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E8">
-        <v>2.95</v>
+        <v>0.63</v>
       </c>
       <c r="F8">
-        <v>4.04</v>
+        <v>3.2</v>
       </c>
       <c r="G8">
-        <v>-5.58</v>
+        <v>5.85</v>
       </c>
       <c r="H8">
-        <v>7.77</v>
+        <v>-3.54</v>
       </c>
       <c r="I8">
-        <v>-0.23</v>
-      </c>
-      <c r="J8">
-        <v>-6.79</v>
-      </c>
-      <c r="K8">
-        <v>-4.75</v>
-      </c>
-      <c r="L8">
-        <v>-7.02</v>
-      </c>
-      <c r="M8">
-        <v>-6.37</v>
-      </c>
-      <c r="N8">
-        <v>-2.31</v>
-      </c>
-      <c r="O8">
-        <v>-5.15</v>
-      </c>
-      <c r="P8">
-        <v>-3.67</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>69356V971439</t>
+          <t>00381V249612</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Glemmen</t>
+          <t>Ellingsøytunnelen sør</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>fv. 109</t>
+          <t>rv. 658</t>
         </is>
       </c>
       <c r="D9">
         <v>2025</v>
       </c>
       <c r="E9">
-        <v>-2.66</v>
+        <v>-1.97</v>
       </c>
       <c r="F9">
-        <v>-5.1</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>3.97</v>
+        <v>2.06</v>
       </c>
       <c r="H9">
-        <v>-4.51</v>
+        <v>-4.62</v>
       </c>
       <c r="I9">
-        <v>0.86</v>
-      </c>
-      <c r="J9">
-        <v>0.26</v>
+        <v>-0.12</v>
       </c>
       <c r="K9">
-        <v>0.52</v>
+        <v>7.43</v>
       </c>
       <c r="L9">
-        <v>1.25</v>
+        <v>1.22</v>
       </c>
       <c r="M9">
-        <v>3.03</v>
+        <v>2.61</v>
       </c>
       <c r="N9">
-        <v>2.8</v>
+        <v>1.21</v>
+      </c>
+      <c r="O9">
+        <v>-1.03</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>07156V971848</t>
+          <t>55272V248971</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Grøte bru</t>
+          <t>Emblem</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>fv. 581</t>
+          <t>fv. 60</t>
         </is>
       </c>
       <c r="D10">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E10">
-        <v>-3.35</v>
+        <v>1.22</v>
       </c>
       <c r="F10">
-        <v>-0.4</v>
+        <v>-0.01</v>
       </c>
       <c r="G10">
-        <v>-7.44</v>
+        <v>-0.21</v>
       </c>
       <c r="H10">
-        <v>1.1</v>
+        <v>0.24</v>
       </c>
       <c r="I10">
-        <v>-8.699999999999999</v>
+        <v>2.73</v>
+      </c>
+      <c r="J10">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="K10">
+        <v>0.35</v>
       </c>
       <c r="L10">
-        <v>-5.13</v>
-      </c>
-      <c r="M10">
-        <v>-6.71</v>
-      </c>
-      <c r="N10">
-        <v>-4.43</v>
+        <v>-1.83</v>
       </c>
       <c r="O10">
-        <v>-4.61</v>
-      </c>
-      <c r="P10">
-        <v>-2.45</v>
+        <v>-0.57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>07156V971848</t>
+          <t>62667V249427</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Grøte bru</t>
+          <t>Høgvollstubben</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>fv. 581</t>
+          <t>fv. 534</t>
         </is>
       </c>
       <c r="D11">
         <v>2025</v>
       </c>
       <c r="E11">
-        <v>-1.31</v>
+        <v>-0.62</v>
       </c>
       <c r="F11">
-        <v>-3.39</v>
+        <v>0.52</v>
       </c>
       <c r="G11">
-        <v>4.79</v>
+        <v>3.21</v>
       </c>
       <c r="H11">
-        <v>1.11</v>
+        <v>-5.64</v>
       </c>
       <c r="I11">
-        <v>10.09</v>
+        <v>2.42</v>
       </c>
       <c r="J11">
-        <v>5.52</v>
-      </c>
-      <c r="K11">
-        <v>7.58</v>
-      </c>
-      <c r="L11">
-        <v>4.86</v>
-      </c>
-      <c r="M11">
-        <v>5.98</v>
-      </c>
-      <c r="N11">
-        <v>5.51</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>88954V971483</t>
+          <t>85413V249430</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hafslund sør</t>
+          <t>Kolvikbakken ungdomskole</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>rv. 22</t>
+          <t>fv. 536</t>
         </is>
       </c>
       <c r="D12">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E12">
-        <v>-1.21</v>
+        <v>2.39</v>
       </c>
       <c r="F12">
-        <v>1.11</v>
+        <v>3.85</v>
       </c>
       <c r="G12">
-        <v>-5.45</v>
+        <v>7.2</v>
       </c>
       <c r="H12">
-        <v>-1.37</v>
+        <v>-10.06</v>
       </c>
       <c r="I12">
-        <v>-11.03</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="J12">
-        <v>-13.19</v>
-      </c>
-      <c r="K12">
-        <v>-9.18</v>
-      </c>
-      <c r="L12">
-        <v>-9.210000000000001</v>
-      </c>
-      <c r="M12">
-        <v>-9.130000000000001</v>
-      </c>
-      <c r="N12">
-        <v>-7.04</v>
-      </c>
-      <c r="O12">
-        <v>-7.91</v>
-      </c>
-      <c r="P12">
-        <v>-6.61</v>
+        <v>-0.28</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>88954V971483</t>
+          <t>58348V248957</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hafslund sør</t>
+          <t>Lerstad - Volsdalen</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>rv. 22</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D13">
         <v>2025</v>
       </c>
       <c r="E13">
-        <v>-3.11</v>
+        <v>4.1</v>
       </c>
       <c r="F13">
-        <v>-6.38</v>
+        <v>2.07</v>
       </c>
       <c r="G13">
-        <v>0.28</v>
+        <v>7.92</v>
       </c>
       <c r="H13">
-        <v>-1.22</v>
+        <v>-9.470000000000001</v>
       </c>
       <c r="I13">
-        <v>3.58</v>
+        <v>2.29</v>
       </c>
       <c r="J13">
-        <v>3.42</v>
+        <v>3.72</v>
       </c>
       <c r="K13">
-        <v>4.51</v>
+        <v>1.85</v>
       </c>
       <c r="L13">
-        <v>-0.99</v>
+        <v>-2.46</v>
       </c>
       <c r="M13">
-        <v>-0.99</v>
+        <v>-1.03</v>
       </c>
       <c r="N13">
-        <v>-0.2</v>
+        <v>-4.41</v>
+      </c>
+      <c r="O13">
+        <v>-6.35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>87740V971816</t>
+          <t>82819V248945</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Hafslund øst</t>
+          <t>Moa nord</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>rv. 22</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D14">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E14">
-        <v>-8.619999999999999</v>
+        <v>3.67</v>
       </c>
       <c r="F14">
-        <v>-5.06</v>
+        <v>1.68</v>
       </c>
       <c r="G14">
-        <v>-10.76</v>
+        <v>5.46</v>
       </c>
       <c r="H14">
-        <v>-0.63</v>
+        <v>-1.83</v>
       </c>
       <c r="I14">
-        <v>-3.76</v>
+        <v>4.56</v>
       </c>
       <c r="J14">
-        <v>-6.5</v>
-      </c>
-      <c r="K14">
-        <v>-6.1</v>
-      </c>
-      <c r="L14">
-        <v>-7.58</v>
-      </c>
-      <c r="M14">
-        <v>-8.08</v>
-      </c>
-      <c r="N14">
-        <v>-4.18</v>
-      </c>
-      <c r="O14">
-        <v>-3.58</v>
-      </c>
-      <c r="P14">
-        <v>-1.2</v>
+        <v>2.55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>87740V971816</t>
+          <t>06164V248948</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hafslund øst</t>
+          <t>Moa vest</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>rv. 22</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D15">
         <v>2025</v>
       </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>3.61</v>
+      </c>
+      <c r="G15">
+        <v>7.47</v>
+      </c>
+      <c r="H15">
+        <v>-3.35</v>
+      </c>
+      <c r="I15">
+        <v>4.73</v>
+      </c>
+      <c r="J15">
+        <v>-0.03</v>
+      </c>
+      <c r="K15">
+        <v>-1.53</v>
+      </c>
+      <c r="L15">
+        <v>-0.71</v>
+      </c>
+      <c r="M15">
+        <v>0.99</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>96583V971490</t>
+          <t>54426V248907</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Hauge bru</t>
+          <t>Moatunnelen</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>fv. 112</t>
+          <t>E39</t>
         </is>
       </c>
       <c r="D16">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E16">
-        <v>-2.5</v>
+        <v>2.74</v>
       </c>
       <c r="F16">
-        <v>2.14</v>
+        <v>1.7</v>
       </c>
       <c r="G16">
-        <v>-6.75</v>
+        <v>6.15</v>
       </c>
       <c r="H16">
-        <v>12.6</v>
+        <v>-2.47</v>
       </c>
       <c r="I16">
-        <v>-1.16</v>
+        <v>2.8</v>
       </c>
       <c r="J16">
-        <v>-3.07</v>
-      </c>
-      <c r="K16">
-        <v>0.11</v>
-      </c>
-      <c r="L16">
-        <v>-1.85</v>
-      </c>
-      <c r="M16">
-        <v>-1.93</v>
-      </c>
-      <c r="N16">
-        <v>3.58</v>
-      </c>
-      <c r="O16">
-        <v>-0.37</v>
-      </c>
-      <c r="P16">
-        <v>2.48</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>96583V971490</t>
+          <t>38589V248954</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Hauge bru</t>
+          <t>Nørvasundet arm Borgundvegen-Moa</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>fv. 112</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D17">
         <v>2025</v>
       </c>
+      <c r="E17">
+        <v>8.390000000000001</v>
+      </c>
       <c r="F17">
-        <v>-0.87</v>
+        <v>7.5</v>
       </c>
       <c r="G17">
-        <v>7.51</v>
+        <v>13.1</v>
       </c>
       <c r="H17">
-        <v>-4.04</v>
+        <v>-0.62</v>
       </c>
       <c r="I17">
+        <v>7.76</v>
+      </c>
+      <c r="J17">
+        <v>2.2</v>
+      </c>
+      <c r="K17">
         <v>3.76</v>
       </c>
-      <c r="J17">
-        <v>-0.06</v>
-      </c>
-      <c r="K17">
-        <v>1.31</v>
-      </c>
       <c r="L17">
-        <v>0.15</v>
-      </c>
-      <c r="M17">
-        <v>0.26</v>
-      </c>
-      <c r="N17">
-        <v>-0.8</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>71595V971806</t>
+          <t>85956V248955</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hvitsten</t>
+          <t>Nørvasundet arm Ålesund-Borgundvegen</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>rv. 22</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D18">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E18">
-        <v>-1.49</v>
+        <v>-4.26</v>
       </c>
       <c r="F18">
-        <v>-0.93</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="G18">
-        <v>-9.99</v>
+        <v>2.41</v>
       </c>
       <c r="H18">
-        <v>2.21</v>
+        <v>-7.25</v>
       </c>
       <c r="I18">
-        <v>-5.25</v>
+        <v>-1.02</v>
       </c>
       <c r="J18">
-        <v>-7.92</v>
+        <v>1.08</v>
       </c>
       <c r="K18">
-        <v>-6.96</v>
+        <v>5.76</v>
       </c>
       <c r="L18">
-        <v>-5.48</v>
-      </c>
-      <c r="M18">
-        <v>-5.33</v>
-      </c>
-      <c r="N18">
-        <v>-0.46</v>
-      </c>
-      <c r="O18">
-        <v>-3.09</v>
-      </c>
-      <c r="P18">
-        <v>-4.15</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>71595V971806</t>
+          <t>09421V248956</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hvitsten</t>
+          <t>Nørvasundet nord Borgund - Ålesund</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>rv. 22</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D19">
         <v>2025</v>
       </c>
       <c r="E19">
-        <v>-2.65</v>
+        <v>-3.18</v>
       </c>
       <c r="F19">
-        <v>-4.83</v>
+        <v>-2.53</v>
       </c>
       <c r="G19">
-        <v>4.38</v>
+        <v>0.61</v>
       </c>
       <c r="H19">
-        <v>8.630000000000001</v>
+        <v>-9.279999999999999</v>
       </c>
       <c r="I19">
-        <v>6.06</v>
+        <v>-1.02</v>
       </c>
       <c r="J19">
-        <v>7.36</v>
+        <v>-0.25</v>
       </c>
       <c r="K19">
-        <v>4.08</v>
-      </c>
-      <c r="L19">
-        <v>2.83</v>
-      </c>
-      <c r="M19">
-        <v>4.97</v>
-      </c>
-      <c r="N19">
-        <v>1.02</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>82913V971429</t>
+          <t>41170V248953</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kråkerøy bru</t>
+          <t>Nørvasundet nord Lerstad - Borgund</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>fv. 108</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D20">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E20">
-        <v>4.36</v>
+        <v>6.25</v>
       </c>
       <c r="F20">
-        <v>8.09</v>
+        <v>7.29</v>
       </c>
       <c r="G20">
-        <v>-0.87</v>
+        <v>14.74</v>
       </c>
       <c r="H20">
-        <v>9.210000000000001</v>
+        <v>-1.94</v>
       </c>
       <c r="I20">
-        <v>8.26</v>
+        <v>6</v>
       </c>
       <c r="J20">
-        <v>3.65</v>
+        <v>1.45</v>
       </c>
       <c r="K20">
-        <v>0.14</v>
-      </c>
-      <c r="L20">
-        <v>-6.58</v>
-      </c>
-      <c r="M20">
-        <v>-6.17</v>
-      </c>
-      <c r="N20">
-        <v>0.29</v>
-      </c>
-      <c r="O20">
-        <v>2.9</v>
-      </c>
-      <c r="P20">
-        <v>8.789999999999999</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>82913V971429</t>
+          <t>33030V248950</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kråkerøy bru</t>
+          <t>Skuggentunnelen</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>fv. 108</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D21">
         <v>2025</v>
       </c>
       <c r="E21">
-        <v>7.16</v>
-      </c>
-      <c r="F21">
-        <v>5.26</v>
+        <v>2.16</v>
       </c>
       <c r="G21">
-        <v>13.45</v>
+        <v>6.9</v>
       </c>
       <c r="H21">
-        <v>8.470000000000001</v>
+        <v>-3.61</v>
       </c>
       <c r="I21">
-        <v>7.56</v>
+        <v>3.46</v>
       </c>
       <c r="J21">
-        <v>6.86</v>
+        <v>0.31</v>
       </c>
       <c r="K21">
-        <v>10.79</v>
-      </c>
-      <c r="M21">
-        <v>8.470000000000001</v>
-      </c>
-      <c r="N21">
-        <v>12.73</v>
+        <v>1.9</v>
+      </c>
+      <c r="L21">
+        <v>0.08</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>45854V971841</t>
+          <t>65035V248952</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nordre Veum</t>
+          <t>Skutvika</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>fv. 381</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D22">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E22">
-        <v>-17.94</v>
+        <v>-1.32</v>
       </c>
       <c r="F22">
-        <v>-11.45</v>
+        <v>1.13</v>
       </c>
       <c r="G22">
-        <v>-17.59</v>
+        <v>2.18</v>
       </c>
       <c r="H22">
-        <v>0.11</v>
+        <v>-2.22</v>
       </c>
       <c r="I22">
-        <v>-11.76</v>
+        <v>3.18</v>
       </c>
       <c r="J22">
-        <v>-11.03</v>
+        <v>1.99</v>
       </c>
       <c r="K22">
-        <v>-9.039999999999999</v>
+        <v>3.86</v>
       </c>
       <c r="L22">
-        <v>-10.93</v>
+        <v>3.45</v>
+      </c>
+      <c r="M22">
+        <v>4.47</v>
       </c>
       <c r="N22">
-        <v>-2.89</v>
+        <v>4.28</v>
       </c>
       <c r="O22">
-        <v>-5.3</v>
-      </c>
-      <c r="P22">
-        <v>4.18</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>45854V971841</t>
+          <t>16467V249421</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Nordre Veum</t>
+          <t>Spjelkavik sør</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>fv. 381</t>
+          <t>fv. 6210</t>
         </is>
       </c>
       <c r="D23">
         <v>2025</v>
       </c>
+      <c r="E23">
+        <v>-3.58</v>
+      </c>
       <c r="F23">
-        <v>-5.23</v>
+        <v>-1.81</v>
       </c>
       <c r="G23">
-        <v>5.37</v>
+        <v>6.39</v>
       </c>
       <c r="H23">
-        <v>-5.36</v>
+        <v>-5.65</v>
       </c>
       <c r="I23">
-        <v>-1.7</v>
+        <v>-2.37</v>
       </c>
       <c r="J23">
-        <v>2.64</v>
+        <v>4.82</v>
       </c>
       <c r="K23">
-        <v>0.76</v>
+        <v>-0.87</v>
       </c>
       <c r="L23">
-        <v>-0.06</v>
-      </c>
-      <c r="N23">
-        <v>-2.52</v>
+        <v>-3.91</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>31043V971805</t>
+          <t>75571V248950</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Rakkestadsvingen nord</t>
+          <t>Volsdalen</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>rv. 22</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D24">
-        <v>2024</v>
+        <v>2025</v>
+      </c>
+      <c r="E24">
+        <v>-0.62</v>
+      </c>
+      <c r="F24">
+        <v>1.4</v>
       </c>
       <c r="G24">
-        <v>-3.64</v>
+        <v>5.26</v>
       </c>
       <c r="H24">
-        <v>7.13</v>
+        <v>-4.71</v>
       </c>
       <c r="I24">
-        <v>1.76</v>
+        <v>2.11</v>
       </c>
       <c r="J24">
-        <v>-4.36</v>
+        <v>0.14</v>
       </c>
       <c r="K24">
-        <v>-2.5</v>
+        <v>2.63</v>
       </c>
       <c r="L24">
-        <v>-1.67</v>
+        <v>0.43</v>
       </c>
       <c r="M24">
-        <v>3.28</v>
+        <v>2.4</v>
       </c>
       <c r="N24">
-        <v>6.65</v>
+        <v>0.91</v>
       </c>
       <c r="O24">
-        <v>1.04</v>
-      </c>
-      <c r="P24">
-        <v>1.38</v>
+        <v>-0.67</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>31043V971805</t>
+          <t>23347V248958</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Rakkestadsvingen nord</t>
+          <t>Volsdalen - Lerstad</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>rv. 22</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D25">
         <v>2025</v>
       </c>
       <c r="E25">
-        <v>2.64</v>
+        <v>2.02</v>
       </c>
       <c r="F25">
-        <v>-0.74</v>
+        <v>0.37</v>
       </c>
       <c r="G25">
-        <v>6.14</v>
+        <v>6.07</v>
       </c>
       <c r="H25">
-        <v>-1.33</v>
+        <v>-10.82</v>
       </c>
       <c r="I25">
-        <v>2.16</v>
+        <v>3.52</v>
       </c>
       <c r="J25">
-        <v>7.46</v>
+        <v>2.89</v>
       </c>
       <c r="K25">
-        <v>3.65</v>
+        <v>2.23</v>
       </c>
       <c r="L25">
-        <v>1.86</v>
+        <v>-0.13</v>
       </c>
       <c r="M25">
-        <v>-2.07</v>
+        <v>0.23</v>
       </c>
       <c r="N25">
-        <v>-3.08</v>
+        <v>-3.07</v>
+      </c>
+      <c r="O25">
+        <v>-6.03</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06966V971804</t>
+          <t>81077V248960</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Rakkestadsvingen øst</t>
+          <t xml:space="preserve">Volsdalen rampearm </t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>fv. 130</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D26">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E26">
-        <v>-4.93</v>
+        <v>-2.11</v>
       </c>
       <c r="F26">
-        <v>-0.53</v>
+        <v>2.05</v>
       </c>
       <c r="G26">
-        <v>-3.97</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="H26">
-        <v>4.16</v>
+        <v>-9.42</v>
       </c>
       <c r="I26">
-        <v>0.84</v>
+        <v>1.52</v>
       </c>
       <c r="J26">
-        <v>-3.1</v>
+        <v>1.53</v>
       </c>
       <c r="K26">
-        <v>-3.67</v>
+        <v>3.7</v>
       </c>
       <c r="L26">
-        <v>-0.46</v>
+        <v>-0.32</v>
       </c>
       <c r="M26">
-        <v>-5.44</v>
+        <v>5.71</v>
       </c>
       <c r="N26">
-        <v>-3.51</v>
+        <v>4.35</v>
       </c>
       <c r="O26">
-        <v>1.1</v>
-      </c>
-      <c r="P26">
-        <v>4.28</v>
+        <v>4.87</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06966V971804</t>
+          <t>63171V248950</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Rakkestadsvingen øst</t>
+          <t>Volsdalen øst</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>fv. 130</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D27">
         <v>2025</v>
       </c>
       <c r="E27">
-        <v>7.4</v>
+        <v>-0.93</v>
       </c>
       <c r="F27">
-        <v>6.49</v>
+        <v>0.91</v>
       </c>
       <c r="G27">
-        <v>9.93</v>
+        <v>4.33</v>
       </c>
       <c r="H27">
-        <v>4.81</v>
+        <v>-3.63</v>
       </c>
       <c r="I27">
-        <v>3.62</v>
+        <v>2.1</v>
       </c>
       <c r="J27">
-        <v>4.71</v>
+        <v>-0.35</v>
       </c>
       <c r="K27">
-        <v>8.279999999999999</v>
+        <v>2.19</v>
       </c>
       <c r="L27">
-        <v>4.44</v>
+        <v>0.2</v>
       </c>
       <c r="M27">
-        <v>6.64</v>
+        <v>1.72</v>
       </c>
       <c r="N27">
-        <v>8.869999999999999</v>
+        <v>0.41</v>
+      </c>
+      <c r="O27">
+        <v>-1.75</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>26581V971445</t>
+          <t>07156V248908</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Rolvsøysund bru</t>
+          <t>Ytterholen</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>fv. 109</t>
+          <t>E39</t>
         </is>
       </c>
       <c r="D28">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E28">
-        <v>-4</v>
+        <v>4.36</v>
       </c>
       <c r="F28">
-        <v>-0.63</v>
+        <v>2.06</v>
       </c>
       <c r="G28">
-        <v>-10.16</v>
+        <v>2.96</v>
       </c>
       <c r="H28">
-        <v>2.66</v>
+        <v>3.34</v>
       </c>
       <c r="I28">
-        <v>1.47</v>
-      </c>
-      <c r="J28">
-        <v>-3.96</v>
-      </c>
-      <c r="K28">
-        <v>-6.22</v>
-      </c>
-      <c r="L28">
-        <v>-6.27</v>
-      </c>
-      <c r="M28">
-        <v>-7.15</v>
-      </c>
-      <c r="N28">
-        <v>-2.41</v>
-      </c>
-      <c r="O28">
-        <v>-2.01</v>
-      </c>
-      <c r="P28">
-        <v>-2.22</v>
+        <v>6.21</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>26581V971445</t>
+          <t>67715V248950</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Rolvsøysund bru</t>
+          <t>Ålesund - Volsdalen</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>fv. 109</t>
+          <t>E136</t>
         </is>
       </c>
       <c r="D29">
         <v>2025</v>
       </c>
       <c r="E29">
-        <v>0.06</v>
+        <v>3.83</v>
       </c>
       <c r="F29">
-        <v>-5.3</v>
+        <v>5.89</v>
       </c>
       <c r="G29">
-        <v>3.32</v>
+        <v>13.05</v>
       </c>
       <c r="H29">
-        <v>-3.52</v>
+        <v>-8.57</v>
       </c>
       <c r="I29">
-        <v>0.88</v>
+        <v>3</v>
       </c>
       <c r="J29">
-        <v>0.48</v>
+        <v>3.4</v>
       </c>
       <c r="K29">
-        <v>2.66</v>
+        <v>7.14</v>
       </c>
       <c r="L29">
-        <v>0.4</v>
+        <v>2.39</v>
       </c>
       <c r="M29">
-        <v>3.21</v>
+        <v>5.17</v>
       </c>
       <c r="N29">
-        <v>-0.49</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>16035V971817</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Sarpsfossen bru</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>fv. 118</t>
-        </is>
-      </c>
-      <c r="D30">
-        <v>2024</v>
-      </c>
-      <c r="E30">
-        <v>-5.98</v>
-      </c>
-      <c r="F30">
-        <v>-3.05</v>
-      </c>
-      <c r="G30">
-        <v>-11.44</v>
-      </c>
-      <c r="H30">
-        <v>-4.75</v>
-      </c>
-      <c r="I30">
-        <v>-10.67</v>
-      </c>
-      <c r="J30">
-        <v>-12.98</v>
-      </c>
-      <c r="K30">
-        <v>-11.76</v>
-      </c>
-      <c r="L30">
-        <v>-11.53</v>
-      </c>
-      <c r="M30">
-        <v>-10.24</v>
-      </c>
-      <c r="N30">
-        <v>-7.83</v>
-      </c>
-      <c r="O30">
-        <v>-8.109999999999999</v>
-      </c>
-      <c r="P30">
-        <v>-6.35</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>16035V971817</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Sarpsfossen bru</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>fv. 118</t>
-        </is>
-      </c>
-      <c r="D31">
-        <v>2025</v>
-      </c>
-      <c r="E31">
-        <v>-3.42</v>
-      </c>
-      <c r="F31">
-        <v>-7.79</v>
-      </c>
-      <c r="G31">
-        <v>0.82</v>
-      </c>
-      <c r="H31">
-        <v>-1.81</v>
-      </c>
-      <c r="I31">
-        <v>2.39</v>
-      </c>
-      <c r="J31">
-        <v>3.93</v>
-      </c>
-      <c r="K31">
-        <v>3.44</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>0.55</v>
-      </c>
-      <c r="N31">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>05882V3188133</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Simo</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>rv. 110</t>
-        </is>
-      </c>
-      <c r="D32">
-        <v>2024</v>
-      </c>
-      <c r="E32">
-        <v>2.19</v>
-      </c>
-      <c r="F32">
-        <v>6.41</v>
-      </c>
-      <c r="G32">
-        <v>0.25</v>
-      </c>
-      <c r="H32">
-        <v>7.09</v>
-      </c>
-      <c r="I32">
-        <v>2.58</v>
-      </c>
-      <c r="J32">
-        <v>-5.42</v>
-      </c>
-      <c r="K32">
-        <v>-2.88</v>
-      </c>
-      <c r="L32">
-        <v>-1.47</v>
-      </c>
-      <c r="M32">
-        <v>-2.76</v>
-      </c>
-      <c r="N32">
-        <v>0.54</v>
-      </c>
-      <c r="O32">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="P32">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>05882V3188133</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Simo</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>rv. 110</t>
-        </is>
-      </c>
-      <c r="D33">
-        <v>2025</v>
-      </c>
-      <c r="E33">
-        <v>2.73</v>
-      </c>
-      <c r="F33">
-        <v>-2.04</v>
-      </c>
-      <c r="G33">
-        <v>4.87</v>
-      </c>
-      <c r="H33">
-        <v>1.95</v>
-      </c>
-      <c r="I33">
-        <v>1.17</v>
-      </c>
-      <c r="J33">
-        <v>5.02</v>
-      </c>
-      <c r="K33">
-        <v>5.94</v>
-      </c>
-      <c r="L33">
-        <v>2.04</v>
-      </c>
-      <c r="M33">
-        <v>2.47</v>
-      </c>
-      <c r="N33">
-        <v>2.66</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>13990V971815</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Skjeberg nord</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>fv. 118</t>
-        </is>
-      </c>
-      <c r="D34">
-        <v>2024</v>
-      </c>
-      <c r="E34">
-        <v>-0.54</v>
-      </c>
-      <c r="F34">
-        <v>2.3</v>
-      </c>
-      <c r="G34">
-        <v>3.57</v>
-      </c>
-      <c r="H34">
-        <v>10.09</v>
-      </c>
-      <c r="I34">
-        <v>10.07</v>
-      </c>
-      <c r="J34">
-        <v>0.83</v>
-      </c>
-      <c r="K34">
-        <v>10.22</v>
-      </c>
-      <c r="L34">
-        <v>9.66</v>
-      </c>
-      <c r="N34">
-        <v>10.12</v>
-      </c>
-      <c r="O34">
-        <v>6.73</v>
-      </c>
-      <c r="P34">
-        <v>11.93</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>13990V971815</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Skjeberg nord</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>fv. 118</t>
-        </is>
-      </c>
-      <c r="D35">
-        <v>2025</v>
-      </c>
-      <c r="E35">
-        <v>9.109999999999999</v>
-      </c>
-      <c r="F35">
-        <v>6.79</v>
-      </c>
-      <c r="G35">
-        <v>8.779999999999999</v>
-      </c>
-      <c r="H35">
-        <v>2.81</v>
-      </c>
-      <c r="I35">
-        <v>-2.87</v>
-      </c>
-      <c r="J35">
-        <v>1.44</v>
-      </c>
-      <c r="K35">
-        <v>8.640000000000001</v>
-      </c>
-      <c r="L35">
-        <v>2.23</v>
-      </c>
-      <c r="N35">
-        <v>-0.03</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>92069V971506</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Skåra</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>fv. 116</t>
-        </is>
-      </c>
-      <c r="D36">
-        <v>2024</v>
-      </c>
-      <c r="E36">
-        <v>-2.07</v>
-      </c>
-      <c r="F36">
-        <v>3.14</v>
-      </c>
-      <c r="G36">
-        <v>-1.31</v>
-      </c>
-      <c r="H36">
-        <v>7.47</v>
-      </c>
-      <c r="I36">
-        <v>3.17</v>
-      </c>
-      <c r="J36">
-        <v>-4.55</v>
-      </c>
-      <c r="K36">
-        <v>-0.51</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
-      <c r="O36">
-        <v>-0.5</v>
-      </c>
-      <c r="P36">
-        <v>4.41</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>92069V971506</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Skåra</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>fv. 116</t>
-        </is>
-      </c>
-      <c r="D37">
-        <v>2025</v>
-      </c>
-      <c r="E37">
-        <v>4.11</v>
-      </c>
-      <c r="F37">
-        <v>-1.22</v>
-      </c>
-      <c r="G37">
-        <v>5.03</v>
-      </c>
-      <c r="H37">
-        <v>0.83</v>
-      </c>
-      <c r="I37">
-        <v>1.64</v>
-      </c>
-      <c r="J37">
-        <v>3.83</v>
-      </c>
-      <c r="K37">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="L37">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>54674V971471</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Solberg vest</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>fv. 130</t>
-        </is>
-      </c>
-      <c r="D38">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>54674V971471</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Solberg vest</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>fv. 130</t>
-        </is>
-      </c>
-      <c r="D39">
-        <v>2025</v>
-      </c>
-      <c r="K39">
-        <v>9.720000000000001</v>
-      </c>
-      <c r="L39">
-        <v>5.72</v>
-      </c>
-      <c r="M39">
-        <v>4.6</v>
-      </c>
-      <c r="N39">
-        <v>4.99</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>86688V971471</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Solberg øst</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>fv. 130</t>
-        </is>
-      </c>
-      <c r="D40">
-        <v>2024</v>
-      </c>
-      <c r="E40">
-        <v>5.64</v>
-      </c>
-      <c r="F40">
-        <v>8.119999999999999</v>
-      </c>
-      <c r="G40">
-        <v>6.62</v>
-      </c>
-      <c r="H40">
-        <v>9.369999999999999</v>
-      </c>
-      <c r="I40">
-        <v>7.43</v>
-      </c>
-      <c r="J40">
-        <v>-5.77</v>
-      </c>
-      <c r="K40">
-        <v>5.82</v>
-      </c>
-      <c r="L40">
-        <v>5.71</v>
-      </c>
-      <c r="M40">
-        <v>-0.9</v>
-      </c>
-      <c r="N40">
-        <v>0.22</v>
-      </c>
-      <c r="O40">
-        <v>-0.5600000000000001</v>
-      </c>
-      <c r="P40">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>86688V971471</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Solberg øst</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>fv. 130</t>
-        </is>
-      </c>
-      <c r="D41">
-        <v>2025</v>
-      </c>
-      <c r="E41">
-        <v>-0.28</v>
-      </c>
-      <c r="F41">
-        <v>-1.86</v>
-      </c>
-      <c r="G41">
-        <v>2.12</v>
-      </c>
-      <c r="H41">
-        <v>1.29</v>
-      </c>
-      <c r="I41">
-        <v>-6.63</v>
-      </c>
-      <c r="J41">
-        <v>0.25</v>
-      </c>
-      <c r="K41">
-        <v>13.09</v>
-      </c>
-      <c r="L41">
-        <v>0.36</v>
-      </c>
-      <c r="M41">
-        <v>0.99</v>
-      </c>
-      <c r="N41">
-        <v>4.09</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>29937V971442</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Stabburet</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>fv. 109</t>
-        </is>
-      </c>
-      <c r="D42">
-        <v>2024</v>
-      </c>
-      <c r="E42">
-        <v>6.35</v>
-      </c>
-      <c r="F42">
-        <v>6.78</v>
-      </c>
-      <c r="G42">
-        <v>-2.94</v>
-      </c>
-      <c r="H42">
-        <v>9.44</v>
-      </c>
-      <c r="I42">
-        <v>1.36</v>
-      </c>
-      <c r="J42">
-        <v>-5.96</v>
-      </c>
-      <c r="K42">
-        <v>-4.27</v>
-      </c>
-      <c r="L42">
-        <v>-6</v>
-      </c>
-      <c r="M42">
-        <v>-4.74</v>
-      </c>
-      <c r="N42">
-        <v>-1.35</v>
-      </c>
-      <c r="O42">
-        <v>-4.85</v>
-      </c>
-      <c r="P42">
-        <v>-4.41</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>29937V971442</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Stabburet</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>fv. 109</t>
-        </is>
-      </c>
-      <c r="D43">
-        <v>2025</v>
-      </c>
-      <c r="E43">
-        <v>-2.85</v>
-      </c>
-      <c r="F43">
-        <v>-5.42</v>
-      </c>
-      <c r="G43">
-        <v>2.81</v>
-      </c>
-      <c r="H43">
-        <v>-4.4</v>
-      </c>
-      <c r="I43">
-        <v>1.05</v>
-      </c>
-      <c r="J43">
-        <v>-0.44</v>
-      </c>
-      <c r="K43">
-        <v>0.51</v>
-      </c>
-      <c r="L43">
-        <v>-1.01</v>
-      </c>
-      <c r="M43">
-        <v>-0.45</v>
-      </c>
-      <c r="N43">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>93031V971807</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Tingvoll</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>fv. 114</t>
-        </is>
-      </c>
-      <c r="D44">
-        <v>2024</v>
-      </c>
-      <c r="E44">
-        <v>-13.07</v>
-      </c>
-      <c r="F44">
-        <v>-9.460000000000001</v>
-      </c>
-      <c r="G44">
-        <v>-10.3</v>
-      </c>
-      <c r="H44">
-        <v>9.98</v>
-      </c>
-      <c r="L44">
-        <v>-5.88</v>
-      </c>
-      <c r="M44">
-        <v>-5.34</v>
-      </c>
-      <c r="N44">
-        <v>-4.37</v>
-      </c>
-      <c r="O44">
-        <v>-2.09</v>
-      </c>
-      <c r="P44">
-        <v>-6.68</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>93031V971807</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Tingvoll</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>fv. 114</t>
-        </is>
-      </c>
-      <c r="D45">
-        <v>2025</v>
-      </c>
-      <c r="E45">
-        <v>2.2</v>
-      </c>
-      <c r="F45">
-        <v>-1.44</v>
-      </c>
-      <c r="G45">
-        <v>1.22</v>
-      </c>
-      <c r="H45">
-        <v>-3.89</v>
-      </c>
-      <c r="I45">
-        <v>-0.34</v>
-      </c>
-      <c r="J45">
-        <v>3.24</v>
-      </c>
-      <c r="K45">
-        <v>5.01</v>
-      </c>
-      <c r="L45">
-        <v>8.140000000000001</v>
-      </c>
-      <c r="M45">
-        <v>6.95</v>
-      </c>
-      <c r="N45">
-        <v>5.54</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>28001V971448</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Torsbekkdalen</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>fv. 109</t>
-        </is>
-      </c>
-      <c r="D46">
-        <v>2024</v>
-      </c>
-      <c r="E46">
-        <v>-1.17</v>
-      </c>
-      <c r="F46">
-        <v>5.26</v>
-      </c>
-      <c r="G46">
-        <v>6.7</v>
-      </c>
-      <c r="H46">
-        <v>18.69</v>
-      </c>
-      <c r="I46">
-        <v>52.17</v>
-      </c>
-      <c r="J46">
-        <v>39.91</v>
-      </c>
-      <c r="K46">
-        <v>9.58</v>
-      </c>
-      <c r="L46">
-        <v>9.52</v>
-      </c>
-      <c r="M46">
-        <v>3.92</v>
-      </c>
-      <c r="N46">
-        <v>7.23</v>
-      </c>
-      <c r="O46">
-        <v>1.63</v>
-      </c>
-      <c r="P46">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>28001V971448</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Torsbekkdalen</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>fv. 109</t>
-        </is>
-      </c>
-      <c r="D47">
-        <v>2025</v>
-      </c>
-      <c r="E47">
-        <v>3.52</v>
-      </c>
-      <c r="F47">
-        <v>-3.81</v>
-      </c>
-      <c r="G47">
-        <v>-10.18</v>
-      </c>
-      <c r="H47">
-        <v>-15.61</v>
-      </c>
-      <c r="I47">
-        <v>-10.44</v>
-      </c>
-      <c r="J47">
-        <v>-9.640000000000001</v>
-      </c>
-      <c r="K47">
-        <v>-6.59</v>
-      </c>
-      <c r="L47">
-        <v>-8.06</v>
-      </c>
-      <c r="M47">
-        <v>-0.87</v>
-      </c>
-      <c r="N47">
-        <v>1.69</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>82998V971817</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Tune kirke</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>fv. 118</t>
-        </is>
-      </c>
-      <c r="D48">
-        <v>2024</v>
-      </c>
-      <c r="E48">
-        <v>-5.76</v>
-      </c>
-      <c r="F48">
-        <v>-3.06</v>
-      </c>
-      <c r="G48">
-        <v>-10.41</v>
-      </c>
-      <c r="H48">
-        <v>-0.29</v>
-      </c>
-      <c r="I48">
-        <v>-13.03</v>
-      </c>
-      <c r="J48">
-        <v>-16.21</v>
-      </c>
-      <c r="K48">
-        <v>-7.98</v>
-      </c>
-      <c r="L48">
-        <v>-9.699999999999999</v>
-      </c>
-      <c r="M48">
-        <v>-7.98</v>
-      </c>
-      <c r="N48">
-        <v>-6.68</v>
-      </c>
-      <c r="O48">
-        <v>-8.220000000000001</v>
-      </c>
-      <c r="P48">
-        <v>-5.26</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>82998V971817</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Tune kirke</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>fv. 118</t>
-        </is>
-      </c>
-      <c r="D49">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>98723V971842</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Veumveien</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>fv. 381</t>
-        </is>
-      </c>
-      <c r="D50">
-        <v>2024</v>
-      </c>
-      <c r="E50">
-        <v>5.92</v>
-      </c>
-      <c r="F50">
-        <v>7.23</v>
-      </c>
-      <c r="G50">
-        <v>-3.77</v>
-      </c>
-      <c r="H50">
-        <v>8.68</v>
-      </c>
-      <c r="I50">
-        <v>-2.65</v>
-      </c>
-      <c r="J50">
-        <v>-11.03</v>
-      </c>
-      <c r="K50">
-        <v>-9.789999999999999</v>
-      </c>
-      <c r="L50">
-        <v>-5.31</v>
-      </c>
-      <c r="M50">
-        <v>-4.5</v>
-      </c>
-      <c r="N50">
-        <v>-3.04</v>
-      </c>
-      <c r="O50">
-        <v>-8.1</v>
-      </c>
-      <c r="P50">
-        <v>-5.06</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>98723V971842</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Veumveien</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>fv. 381</t>
-        </is>
-      </c>
-      <c r="D51">
-        <v>2025</v>
-      </c>
-      <c r="E51">
-        <v>-8</v>
-      </c>
-      <c r="F51">
-        <v>-7.24</v>
-      </c>
-      <c r="G51">
-        <v>-0.14</v>
-      </c>
-      <c r="H51">
-        <v>-4.91</v>
-      </c>
-      <c r="I51">
-        <v>0.13</v>
-      </c>
-      <c r="J51">
-        <v>3.01</v>
-      </c>
-      <c r="K51">
-        <v>0.95</v>
-      </c>
-      <c r="L51">
-        <v>1.93</v>
-      </c>
-      <c r="M51">
-        <v>1.49</v>
-      </c>
-      <c r="N51">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>08132V1984223</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Værstebrua</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>fv. 108</t>
-        </is>
-      </c>
-      <c r="D52">
-        <v>2024</v>
-      </c>
-      <c r="E52">
-        <v>-8.18</v>
-      </c>
-      <c r="F52">
-        <v>-1.68</v>
-      </c>
-      <c r="G52">
-        <v>-7.81</v>
-      </c>
-      <c r="H52">
-        <v>2.56</v>
-      </c>
-      <c r="I52">
-        <v>-7.99</v>
-      </c>
-      <c r="J52">
-        <v>-12.89</v>
-      </c>
-      <c r="K52">
-        <v>-11.65</v>
-      </c>
-      <c r="L52">
-        <v>-8.220000000000001</v>
-      </c>
-      <c r="M52">
-        <v>-7.09</v>
-      </c>
-      <c r="N52">
-        <v>4.61</v>
-      </c>
-      <c r="O52">
-        <v>12.84</v>
-      </c>
-      <c r="P52">
-        <v>17.07</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>08132V1984223</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Værstebrua</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>fv. 108</t>
-        </is>
-      </c>
-      <c r="D53">
-        <v>2025</v>
-      </c>
-      <c r="E53">
-        <v>8.59</v>
-      </c>
-      <c r="F53">
-        <v>10.83</v>
-      </c>
-      <c r="G53">
-        <v>16.02</v>
-      </c>
-      <c r="H53">
-        <v>9.69</v>
-      </c>
-      <c r="I53">
-        <v>12.17</v>
-      </c>
-      <c r="J53">
-        <v>20.97</v>
-      </c>
-      <c r="K53">
-        <v>27.27</v>
-      </c>
-      <c r="M53">
-        <v>19.38</v>
-      </c>
-      <c r="N53">
-        <v>17.48</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>61693V971813</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Ålekilene</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>fv. 117</t>
-        </is>
-      </c>
-      <c r="D54">
-        <v>2024</v>
-      </c>
-      <c r="E54">
-        <v>-2.83</v>
-      </c>
-      <c r="F54">
-        <v>-0.75</v>
-      </c>
-      <c r="G54">
-        <v>-3.1</v>
-      </c>
-      <c r="H54">
-        <v>2.36</v>
-      </c>
-      <c r="I54">
-        <v>1.99</v>
-      </c>
-      <c r="J54">
-        <v>-6.92</v>
-      </c>
-      <c r="K54">
-        <v>-1.06</v>
-      </c>
-      <c r="L54">
-        <v>1.59</v>
-      </c>
-      <c r="N54">
-        <v>1.38</v>
-      </c>
-      <c r="O54">
-        <v>1.6</v>
-      </c>
-      <c r="P54">
-        <v>3.72</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>61693V971813</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Ålekilene</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>fv. 117</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>2025</v>
-      </c>
-      <c r="E55">
-        <v>5.74</v>
-      </c>
-      <c r="F55">
-        <v>1.78</v>
-      </c>
-      <c r="G55">
-        <v>5.56</v>
-      </c>
-      <c r="H55">
-        <v>5.39</v>
-      </c>
-      <c r="I55">
-        <v>0.47</v>
-      </c>
-      <c r="J55">
-        <v>4.75</v>
-      </c>
-      <c r="K55">
-        <v>12.59</v>
-      </c>
-      <c r="L55">
-        <v>1.93</v>
-      </c>
-      <c r="N55">
-        <v>2.14</v>
+        <v>3.34</v>
+      </c>
+      <c r="O29">
+        <v>4.65</v>
       </c>
     </row>
   </sheetData>
@@ -5227,19 +3848,19 @@
         <v>2025</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1.0107</v>
+        <v>1.0098</v>
       </c>
       <c r="F2">
         <v>28</v>
       </c>
       <c r="G2">
-        <v>0.395714491989629</v>
+        <v>0.3965820338959624</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -5258,19 +3879,158 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>okt</t>
+          <t>nov</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>jan-okt</t>
+          <t>jan-nov</t>
         </is>
       </c>
       <c r="M2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="N2">
-        <v>1.9</v>
+        <v>1.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year_base</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>index_p</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>index_i</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>n_trp</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>standard_error</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>index_type</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>year_from_to</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>area_name</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>month_name_short</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ci_lower</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ci_upper</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>2025</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.0098</v>
+      </c>
+      <c r="F2">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>0.3965820338959624</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2024-2025</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Ålesund</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nov</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>jan-nov</t>
+        </is>
+      </c>
+      <c r="M2">
+        <v>0.2</v>
+      </c>
+      <c r="N2">
+        <v>1.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>